<commit_message>
Update BFPIaE for jet fuel
</commit_message>
<xml_diff>
--- a/InputData/fuels/BFPIaE/BAU Fuel Production Imports and Exports.xlsx
+++ b/InputData/fuels/BFPIaE/BAU Fuel Production Imports and Exports.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="5730" tabRatio="684" firstSheet="8" activeTab="15"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="5730" tabRatio="684"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="4" r:id="rId1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="810" uniqueCount="568">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="814" uniqueCount="572">
   <si>
     <t>Source:</t>
   </si>
@@ -1820,6 +1820,18 @@
   </si>
   <si>
     <t>Avg. heat content (Kcal/Kg)</t>
+  </si>
+  <si>
+    <t>Jet fuel</t>
+  </si>
+  <si>
+    <t>production</t>
+  </si>
+  <si>
+    <t>imports</t>
+  </si>
+  <si>
+    <t>exports</t>
   </si>
 </sst>
 </file>
@@ -2520,14 +2532,14 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="15" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="20">
     <cellStyle name="Body: normal cell" xfId="7"/>
@@ -3226,7 +3238,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E158"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
       <selection activeCell="C114" sqref="C114"/>
     </sheetView>
   </sheetViews>
@@ -13939,44 +13951,44 @@
     </row>
     <row r="77" spans="1:37" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="78" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B78" s="93" t="s">
+      <c r="B78" s="96" t="s">
         <v>164</v>
       </c>
-      <c r="C78" s="93"/>
-      <c r="D78" s="93"/>
-      <c r="E78" s="93"/>
-      <c r="F78" s="93"/>
-      <c r="G78" s="93"/>
-      <c r="H78" s="93"/>
-      <c r="I78" s="93"/>
-      <c r="J78" s="93"/>
-      <c r="K78" s="93"/>
-      <c r="L78" s="93"/>
-      <c r="M78" s="93"/>
-      <c r="N78" s="93"/>
-      <c r="O78" s="93"/>
-      <c r="P78" s="93"/>
-      <c r="Q78" s="93"/>
-      <c r="R78" s="93"/>
-      <c r="S78" s="93"/>
-      <c r="T78" s="93"/>
-      <c r="U78" s="93"/>
-      <c r="V78" s="93"/>
-      <c r="W78" s="93"/>
-      <c r="X78" s="93"/>
-      <c r="Y78" s="93"/>
-      <c r="Z78" s="93"/>
-      <c r="AA78" s="93"/>
-      <c r="AB78" s="93"/>
-      <c r="AC78" s="93"/>
-      <c r="AD78" s="93"/>
-      <c r="AE78" s="93"/>
-      <c r="AF78" s="93"/>
-      <c r="AG78" s="93"/>
-      <c r="AH78" s="93"/>
-      <c r="AI78" s="93"/>
-      <c r="AJ78" s="93"/>
-      <c r="AK78" s="93"/>
+      <c r="C78" s="96"/>
+      <c r="D78" s="96"/>
+      <c r="E78" s="96"/>
+      <c r="F78" s="96"/>
+      <c r="G78" s="96"/>
+      <c r="H78" s="96"/>
+      <c r="I78" s="96"/>
+      <c r="J78" s="96"/>
+      <c r="K78" s="96"/>
+      <c r="L78" s="96"/>
+      <c r="M78" s="96"/>
+      <c r="N78" s="96"/>
+      <c r="O78" s="96"/>
+      <c r="P78" s="96"/>
+      <c r="Q78" s="96"/>
+      <c r="R78" s="96"/>
+      <c r="S78" s="96"/>
+      <c r="T78" s="96"/>
+      <c r="U78" s="96"/>
+      <c r="V78" s="96"/>
+      <c r="W78" s="96"/>
+      <c r="X78" s="96"/>
+      <c r="Y78" s="96"/>
+      <c r="Z78" s="96"/>
+      <c r="AA78" s="96"/>
+      <c r="AB78" s="96"/>
+      <c r="AC78" s="96"/>
+      <c r="AD78" s="96"/>
+      <c r="AE78" s="96"/>
+      <c r="AF78" s="96"/>
+      <c r="AG78" s="96"/>
+      <c r="AH78" s="96"/>
+      <c r="AI78" s="96"/>
+      <c r="AJ78" s="96"/>
+      <c r="AK78" s="96"/>
     </row>
     <row r="79" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B79" s="11" t="s">
@@ -16885,8 +16897,8 @@
   </sheetPr>
   <dimension ref="A1:AI23"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView topLeftCell="S1" workbookViewId="0">
+      <selection activeCell="X33" sqref="X33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -18693,140 +18705,140 @@
         <v>30</v>
       </c>
       <c r="B14" s="12">
-        <f>'Petroleum Products'!C13</f>
-        <v>13366862384605.563</v>
+        <f>D14</f>
+        <v>0</v>
       </c>
       <c r="C14">
-        <f t="shared" si="1"/>
-        <v>13366862384605.563</v>
+        <f>D14</f>
+        <v>0</v>
       </c>
       <c r="D14">
-        <f>IF(('BAU Total Primary Fuel Use'!B14-('BFPIaE-production'!D14-'BFPIaE-exports'!D14))&gt;0,('BAU Total Primary Fuel Use'!B14-('BFPIaE-production'!D14-'BFPIaE-exports'!D14)),0)</f>
+        <f>'Petroleum Products'!B31</f>
         <v>0</v>
       </c>
       <c r="E14">
-        <f>IF(('BAU Total Primary Fuel Use'!C14-('BFPIaE-production'!E14-'BFPIaE-exports'!E14))&gt;0,('BAU Total Primary Fuel Use'!C14-('BFPIaE-production'!E14-'BFPIaE-exports'!E14)),0)</f>
+        <f>'Petroleum Products'!C31</f>
         <v>0</v>
       </c>
       <c r="F14">
-        <f>IF(('BAU Total Primary Fuel Use'!D14-('BFPIaE-production'!F14-'BFPIaE-exports'!F14))&gt;0,('BAU Total Primary Fuel Use'!D14-('BFPIaE-production'!F14-'BFPIaE-exports'!F14)),0)</f>
+        <f>'Petroleum Products'!D31</f>
         <v>0</v>
       </c>
       <c r="G14">
-        <f>IF(('BAU Total Primary Fuel Use'!E14-('BFPIaE-production'!G14-'BFPIaE-exports'!G14))&gt;0,('BAU Total Primary Fuel Use'!E14-('BFPIaE-production'!G14-'BFPIaE-exports'!G14)),0)</f>
+        <f>'Petroleum Products'!E31</f>
         <v>0</v>
       </c>
       <c r="H14">
-        <f>IF(('BAU Total Primary Fuel Use'!F14-('BFPIaE-production'!H14-'BFPIaE-exports'!H14))&gt;0,('BAU Total Primary Fuel Use'!F14-('BFPIaE-production'!H14-'BFPIaE-exports'!H14)),0)</f>
+        <f>'Petroleum Products'!F31</f>
         <v>0</v>
       </c>
       <c r="I14">
-        <f>IF(('BAU Total Primary Fuel Use'!G14-('BFPIaE-production'!I14-'BFPIaE-exports'!I14))&gt;0,('BAU Total Primary Fuel Use'!G14-('BFPIaE-production'!I14-'BFPIaE-exports'!I14)),0)</f>
+        <f>'Petroleum Products'!G31</f>
         <v>0</v>
       </c>
       <c r="J14">
-        <f>IF(('BAU Total Primary Fuel Use'!H14-('BFPIaE-production'!J14-'BFPIaE-exports'!J14))&gt;0,('BAU Total Primary Fuel Use'!H14-('BFPIaE-production'!J14-'BFPIaE-exports'!J14)),0)</f>
+        <f>'Petroleum Products'!H31</f>
         <v>0</v>
       </c>
       <c r="K14">
-        <f>IF(('BAU Total Primary Fuel Use'!I14-('BFPIaE-production'!K14-'BFPIaE-exports'!K14))&gt;0,('BAU Total Primary Fuel Use'!I14-('BFPIaE-production'!K14-'BFPIaE-exports'!K14)),0)</f>
+        <f>'Petroleum Products'!I31</f>
         <v>0</v>
       </c>
       <c r="L14">
-        <f>IF(('BAU Total Primary Fuel Use'!J14-('BFPIaE-production'!L14-'BFPIaE-exports'!L14))&gt;0,('BAU Total Primary Fuel Use'!J14-('BFPIaE-production'!L14-'BFPIaE-exports'!L14)),0)</f>
+        <f>'Petroleum Products'!J31</f>
         <v>0</v>
       </c>
       <c r="M14">
-        <f>IF(('BAU Total Primary Fuel Use'!K14-('BFPIaE-production'!M14-'BFPIaE-exports'!M14))&gt;0,('BAU Total Primary Fuel Use'!K14-('BFPIaE-production'!M14-'BFPIaE-exports'!M14)),0)</f>
+        <f>'Petroleum Products'!K31</f>
         <v>0</v>
       </c>
       <c r="N14">
-        <f>IF(('BAU Total Primary Fuel Use'!L14-('BFPIaE-production'!N14-'BFPIaE-exports'!N14))&gt;0,('BAU Total Primary Fuel Use'!L14-('BFPIaE-production'!N14-'BFPIaE-exports'!N14)),0)</f>
+        <f>'Petroleum Products'!L31</f>
         <v>0</v>
       </c>
       <c r="O14">
-        <f>IF(('BAU Total Primary Fuel Use'!M14-('BFPIaE-production'!O14-'BFPIaE-exports'!O14))&gt;0,('BAU Total Primary Fuel Use'!M14-('BFPIaE-production'!O14-'BFPIaE-exports'!O14)),0)</f>
+        <f>'Petroleum Products'!M31</f>
         <v>0</v>
       </c>
       <c r="P14">
-        <f>IF(('BAU Total Primary Fuel Use'!N14-('BFPIaE-production'!P14-'BFPIaE-exports'!P14))&gt;0,('BAU Total Primary Fuel Use'!N14-('BFPIaE-production'!P14-'BFPIaE-exports'!P14)),0)</f>
+        <f>'Petroleum Products'!N31</f>
         <v>0</v>
       </c>
       <c r="Q14">
-        <f>IF(('BAU Total Primary Fuel Use'!O14-('BFPIaE-production'!Q14-'BFPIaE-exports'!Q14))&gt;0,('BAU Total Primary Fuel Use'!O14-('BFPIaE-production'!Q14-'BFPIaE-exports'!Q14)),0)</f>
-        <v>3718384425045.3125</v>
+        <f>'Petroleum Products'!O31</f>
+        <v>0</v>
       </c>
       <c r="R14">
-        <f>IF(('BAU Total Primary Fuel Use'!P14-('BFPIaE-production'!R14-'BFPIaE-exports'!R14))&gt;0,('BAU Total Primary Fuel Use'!P14-('BFPIaE-production'!R14-'BFPIaE-exports'!R14)),0)</f>
-        <v>23839384425045.313</v>
+        <f>'Petroleum Products'!P31</f>
+        <v>0</v>
       </c>
       <c r="S14">
-        <f>IF(('BAU Total Primary Fuel Use'!Q14-('BFPIaE-production'!S14-'BFPIaE-exports'!S14))&gt;0,('BAU Total Primary Fuel Use'!Q14-('BFPIaE-production'!S14-'BFPIaE-exports'!S14)),0)</f>
-        <v>43779384425045.313</v>
+        <f>'Petroleum Products'!Q31</f>
+        <v>0</v>
       </c>
       <c r="T14">
-        <f>IF(('BAU Total Primary Fuel Use'!R14-('BFPIaE-production'!T14-'BFPIaE-exports'!T14))&gt;0,('BAU Total Primary Fuel Use'!R14-('BFPIaE-production'!T14-'BFPIaE-exports'!T14)),0)</f>
-        <v>63691384425045.313</v>
+        <f>'Petroleum Products'!R31</f>
+        <v>0</v>
       </c>
       <c r="U14">
-        <f>IF(('BAU Total Primary Fuel Use'!S14-('BFPIaE-production'!U14-'BFPIaE-exports'!U14))&gt;0,('BAU Total Primary Fuel Use'!S14-('BFPIaE-production'!U14-'BFPIaE-exports'!U14)),0)</f>
-        <v>99967384425045.313</v>
+        <f>'Petroleum Products'!S31</f>
+        <v>0</v>
       </c>
       <c r="V14">
-        <f>IF(('BAU Total Primary Fuel Use'!T14-('BFPIaE-production'!V14-'BFPIaE-exports'!V14))&gt;0,('BAU Total Primary Fuel Use'!T14-('BFPIaE-production'!V14-'BFPIaE-exports'!V14)),0)</f>
-        <v>135929384425045.31</v>
+        <f>'Petroleum Products'!T31</f>
+        <v>0</v>
       </c>
       <c r="W14">
-        <f>IF(('BAU Total Primary Fuel Use'!U14-('BFPIaE-production'!W14-'BFPIaE-exports'!W14))&gt;0,('BAU Total Primary Fuel Use'!U14-('BFPIaE-production'!W14-'BFPIaE-exports'!W14)),0)</f>
-        <v>171422384425045.31</v>
+        <f>'Petroleum Products'!U31</f>
+        <v>0</v>
       </c>
       <c r="X14">
-        <f>IF(('BAU Total Primary Fuel Use'!V14-('BFPIaE-production'!X14-'BFPIaE-exports'!X14))&gt;0,('BAU Total Primary Fuel Use'!V14-('BFPIaE-production'!X14-'BFPIaE-exports'!X14)),0)</f>
-        <v>206497384425045.31</v>
+        <f>'Petroleum Products'!V31</f>
+        <v>0</v>
       </c>
       <c r="Y14">
-        <f>IF(('BAU Total Primary Fuel Use'!W14-('BFPIaE-production'!Y14-'BFPIaE-exports'!Y14))&gt;0,('BAU Total Primary Fuel Use'!W14-('BFPIaE-production'!Y14-'BFPIaE-exports'!Y14)),0)</f>
-        <v>241161384425045.31</v>
+        <f>'Petroleum Products'!W31</f>
+        <v>0</v>
       </c>
       <c r="Z14">
-        <f>IF(('BAU Total Primary Fuel Use'!X14-('BFPIaE-production'!Z14-'BFPIaE-exports'!Z14))&gt;0,('BAU Total Primary Fuel Use'!X14-('BFPIaE-production'!Z14-'BFPIaE-exports'!Z14)),0)</f>
-        <v>286042384425045.31</v>
+        <f>'Petroleum Products'!X31</f>
+        <v>0</v>
       </c>
       <c r="AA14">
-        <f>IF(('BAU Total Primary Fuel Use'!Y14-('BFPIaE-production'!AA14-'BFPIaE-exports'!AA14))&gt;0,('BAU Total Primary Fuel Use'!Y14-('BFPIaE-production'!AA14-'BFPIaE-exports'!AA14)),0)</f>
-        <v>330609384425045.31</v>
+        <f>'Petroleum Products'!Y31</f>
+        <v>663774429781.5</v>
       </c>
       <c r="AB14">
-        <f>IF(('BAU Total Primary Fuel Use'!Z14-('BFPIaE-production'!AB14-'BFPIaE-exports'!AB14))&gt;0,('BAU Total Primary Fuel Use'!Z14-('BFPIaE-production'!AB14-'BFPIaE-exports'!AB14)),0)</f>
-        <v>374820384425045.31</v>
+        <f>'Petroleum Products'!Z31</f>
+        <v>44874774429781.5</v>
       </c>
       <c r="AC14">
-        <f>IF(('BAU Total Primary Fuel Use'!AA14-('BFPIaE-production'!AC14-'BFPIaE-exports'!AC14))&gt;0,('BAU Total Primary Fuel Use'!AA14-('BFPIaE-production'!AC14-'BFPIaE-exports'!AC14)),0)</f>
-        <v>418845384425045.31</v>
+        <f>'Petroleum Products'!AA31</f>
+        <v>88899774429781.5</v>
       </c>
       <c r="AD14">
-        <f>IF(('BAU Total Primary Fuel Use'!AB14-('BFPIaE-production'!AD14-'BFPIaE-exports'!AD14))&gt;0,('BAU Total Primary Fuel Use'!AB14-('BFPIaE-production'!AD14-'BFPIaE-exports'!AD14)),0)</f>
-        <v>462618384425045.31</v>
+        <f>'Petroleum Products'!AB31</f>
+        <v>132672774429781.5</v>
       </c>
       <c r="AE14">
-        <f>IF(('BAU Total Primary Fuel Use'!AC14-('BFPIaE-production'!AE14-'BFPIaE-exports'!AE14))&gt;0,('BAU Total Primary Fuel Use'!AC14-('BFPIaE-production'!AE14-'BFPIaE-exports'!AE14)),0)</f>
-        <v>515397384425045.31</v>
+        <f>'Petroleum Products'!AC31</f>
+        <v>185451774429781.5</v>
       </c>
       <c r="AF14">
-        <f>IF(('BAU Total Primary Fuel Use'!AD14-('BFPIaE-production'!AF14-'BFPIaE-exports'!AF14))&gt;0,('BAU Total Primary Fuel Use'!AD14-('BFPIaE-production'!AF14-'BFPIaE-exports'!AF14)),0)</f>
-        <v>568080384425045.25</v>
+        <f>'Petroleum Products'!AD31</f>
+        <v>238134774429781.5</v>
       </c>
       <c r="AG14">
-        <f>IF(('BAU Total Primary Fuel Use'!AE14-('BFPIaE-production'!AG14-'BFPIaE-exports'!AG14))&gt;0,('BAU Total Primary Fuel Use'!AE14-('BFPIaE-production'!AG14-'BFPIaE-exports'!AG14)),0)</f>
-        <v>620738384425045.25</v>
+        <f>'Petroleum Products'!AE31</f>
+        <v>290792774429781.5</v>
       </c>
       <c r="AH14">
-        <f>IF(('BAU Total Primary Fuel Use'!AF14-('BFPIaE-production'!AH14-'BFPIaE-exports'!AH14))&gt;0,('BAU Total Primary Fuel Use'!AF14-('BFPIaE-production'!AH14-'BFPIaE-exports'!AH14)),0)</f>
-        <v>673231384425045.25</v>
+        <f>'Petroleum Products'!AF31</f>
+        <v>343285774429781.5</v>
       </c>
       <c r="AI14">
-        <f>IF(('BAU Total Primary Fuel Use'!AG14-('BFPIaE-production'!AI14-'BFPIaE-exports'!AI14))&gt;0,('BAU Total Primary Fuel Use'!AG14-('BFPIaE-production'!AI14-'BFPIaE-exports'!AI14)),0)</f>
-        <v>725311384425045.25</v>
+        <f>'Petroleum Products'!AG31</f>
+        <v>395365774429781.5</v>
       </c>
     </row>
     <row r="15" spans="1:35" x14ac:dyDescent="0.45">
@@ -19969,8 +19981,8 @@
   </sheetPr>
   <dimension ref="A1:AI23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="AE27" sqref="AE27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -21610,141 +21622,141 @@
       <c r="A14" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="B14" s="12">
-        <f>'Petroleum Products'!D13</f>
-        <v>329945609995263.81</v>
-      </c>
-      <c r="C14">
-        <f>B14</f>
-        <v>329945609995263.81</v>
-      </c>
-      <c r="D14">
-        <f t="shared" ref="D14:AI14" si="7">C14</f>
-        <v>329945609995263.81</v>
-      </c>
-      <c r="E14">
-        <f t="shared" si="7"/>
-        <v>329945609995263.81</v>
-      </c>
-      <c r="F14">
-        <f t="shared" si="7"/>
-        <v>329945609995263.81</v>
-      </c>
-      <c r="G14">
-        <f t="shared" si="7"/>
-        <v>329945609995263.81</v>
-      </c>
-      <c r="H14">
-        <f t="shared" si="7"/>
-        <v>329945609995263.81</v>
-      </c>
-      <c r="I14">
-        <f t="shared" si="7"/>
-        <v>329945609995263.81</v>
-      </c>
-      <c r="J14">
-        <f t="shared" si="7"/>
-        <v>329945609995263.81</v>
-      </c>
-      <c r="K14">
-        <f t="shared" si="7"/>
-        <v>329945609995263.81</v>
-      </c>
-      <c r="L14">
-        <f t="shared" si="7"/>
-        <v>329945609995263.81</v>
-      </c>
-      <c r="M14">
-        <f t="shared" si="7"/>
-        <v>329945609995263.81</v>
-      </c>
-      <c r="N14">
-        <f t="shared" si="7"/>
-        <v>329945609995263.81</v>
-      </c>
-      <c r="O14">
-        <f t="shared" si="7"/>
-        <v>329945609995263.81</v>
-      </c>
-      <c r="P14">
-        <f t="shared" si="7"/>
-        <v>329945609995263.81</v>
-      </c>
-      <c r="Q14">
-        <f t="shared" si="7"/>
-        <v>329945609995263.81</v>
-      </c>
-      <c r="R14">
-        <f t="shared" si="7"/>
-        <v>329945609995263.81</v>
-      </c>
-      <c r="S14">
-        <f t="shared" si="7"/>
-        <v>329945609995263.81</v>
-      </c>
-      <c r="T14">
-        <f t="shared" si="7"/>
-        <v>329945609995263.81</v>
-      </c>
-      <c r="U14">
-        <f t="shared" si="7"/>
-        <v>329945609995263.81</v>
-      </c>
-      <c r="V14">
-        <f t="shared" si="7"/>
-        <v>329945609995263.81</v>
-      </c>
-      <c r="W14">
-        <f t="shared" si="7"/>
-        <v>329945609995263.81</v>
-      </c>
-      <c r="X14">
-        <f t="shared" si="7"/>
-        <v>329945609995263.81</v>
-      </c>
-      <c r="Y14">
-        <f t="shared" si="7"/>
-        <v>329945609995263.81</v>
-      </c>
-      <c r="Z14">
-        <f t="shared" si="7"/>
-        <v>329945609995263.81</v>
-      </c>
-      <c r="AA14">
-        <f t="shared" si="7"/>
-        <v>329945609995263.81</v>
-      </c>
-      <c r="AB14">
-        <f t="shared" si="7"/>
-        <v>329945609995263.81</v>
-      </c>
-      <c r="AC14">
-        <f t="shared" si="7"/>
-        <v>329945609995263.81</v>
-      </c>
-      <c r="AD14">
-        <f t="shared" si="7"/>
-        <v>329945609995263.81</v>
-      </c>
-      <c r="AE14">
-        <f t="shared" si="7"/>
-        <v>329945609995263.81</v>
-      </c>
-      <c r="AF14">
-        <f t="shared" si="7"/>
-        <v>329945609995263.81</v>
-      </c>
-      <c r="AG14">
-        <f t="shared" si="7"/>
-        <v>329945609995263.81</v>
-      </c>
-      <c r="AH14">
-        <f t="shared" si="7"/>
-        <v>329945609995263.81</v>
-      </c>
-      <c r="AI14">
-        <f t="shared" si="7"/>
-        <v>329945609995263.81</v>
+      <c r="B14" s="31">
+        <f>C14</f>
+        <v>417312225570218.5</v>
+      </c>
+      <c r="C14" s="31">
+        <f>D14</f>
+        <v>417312225570218.5</v>
+      </c>
+      <c r="D14" s="31">
+        <f>'Petroleum Products'!B32</f>
+        <v>417312225570218.5</v>
+      </c>
+      <c r="E14" s="31">
+        <f>'Petroleum Products'!C32</f>
+        <v>479955225570218.5</v>
+      </c>
+      <c r="F14" s="31">
+        <f>'Petroleum Products'!D32</f>
+        <v>482175225570218.5</v>
+      </c>
+      <c r="G14" s="31">
+        <f>'Petroleum Products'!E32</f>
+        <v>492471225570218.5</v>
+      </c>
+      <c r="H14" s="31">
+        <f>'Petroleum Products'!F32</f>
+        <v>476330225570218.5</v>
+      </c>
+      <c r="I14" s="31">
+        <f>'Petroleum Products'!G32</f>
+        <v>462978225570218.5</v>
+      </c>
+      <c r="J14" s="31">
+        <f>'Petroleum Products'!H32</f>
+        <v>451019225570218.5</v>
+      </c>
+      <c r="K14" s="31">
+        <f>'Petroleum Products'!I32</f>
+        <v>433034225570218.5</v>
+      </c>
+      <c r="L14" s="31">
+        <f>'Petroleum Products'!J32</f>
+        <v>415810225570218.5</v>
+      </c>
+      <c r="M14" s="31">
+        <f>'Petroleum Products'!K32</f>
+        <v>399214225570218.5</v>
+      </c>
+      <c r="N14" s="31">
+        <f>'Petroleum Products'!L32</f>
+        <v>383130225570218.5</v>
+      </c>
+      <c r="O14" s="31">
+        <f>'Petroleum Products'!M32</f>
+        <v>367121225570218.5</v>
+      </c>
+      <c r="P14" s="31">
+        <f>'Petroleum Products'!N32</f>
+        <v>346554225570218.5</v>
+      </c>
+      <c r="Q14" s="31">
+        <f>'Petroleum Products'!O32</f>
+        <v>326227225570218.5</v>
+      </c>
+      <c r="R14" s="31">
+        <f>'Petroleum Products'!P32</f>
+        <v>306106225570218.5</v>
+      </c>
+      <c r="S14" s="31">
+        <f>'Petroleum Products'!Q32</f>
+        <v>286166225570218.5</v>
+      </c>
+      <c r="T14" s="31">
+        <f>'Petroleum Products'!R32</f>
+        <v>266254225570218.5</v>
+      </c>
+      <c r="U14" s="31">
+        <f>'Petroleum Products'!S32</f>
+        <v>229978225570218.5</v>
+      </c>
+      <c r="V14" s="31">
+        <f>'Petroleum Products'!T32</f>
+        <v>194016225570218.5</v>
+      </c>
+      <c r="W14" s="31">
+        <f>'Petroleum Products'!U32</f>
+        <v>158523225570218.5</v>
+      </c>
+      <c r="X14" s="31">
+        <f>'Petroleum Products'!V32</f>
+        <v>123448225570218.5</v>
+      </c>
+      <c r="Y14" s="31">
+        <f>'Petroleum Products'!W32</f>
+        <v>88784225570218.5</v>
+      </c>
+      <c r="Z14" s="31">
+        <f>'Petroleum Products'!X32</f>
+        <v>43903225570218.5</v>
+      </c>
+      <c r="AA14" s="31">
+        <f>'Petroleum Products'!Y32</f>
+        <v>0</v>
+      </c>
+      <c r="AB14" s="31">
+        <f>'Petroleum Products'!Z32</f>
+        <v>0</v>
+      </c>
+      <c r="AC14" s="31">
+        <f>'Petroleum Products'!AA32</f>
+        <v>0</v>
+      </c>
+      <c r="AD14" s="31">
+        <f>'Petroleum Products'!AB32</f>
+        <v>0</v>
+      </c>
+      <c r="AE14" s="31">
+        <f>'Petroleum Products'!AC32</f>
+        <v>0</v>
+      </c>
+      <c r="AF14" s="31">
+        <f>'Petroleum Products'!AD32</f>
+        <v>0</v>
+      </c>
+      <c r="AG14" s="31">
+        <f>'Petroleum Products'!AE32</f>
+        <v>0</v>
+      </c>
+      <c r="AH14" s="31">
+        <f>'Petroleum Products'!AF32</f>
+        <v>0</v>
+      </c>
+      <c r="AI14" s="31">
+        <f>'Petroleum Products'!AG32</f>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:35" x14ac:dyDescent="0.45">
@@ -21974,131 +21986,131 @@
         <v>58666666666.666664</v>
       </c>
       <c r="D17">
-        <f t="shared" ref="D17:AI17" si="8">C17</f>
+        <f t="shared" ref="D17:AI17" si="7">C17</f>
         <v>58666666666.666664</v>
       </c>
       <c r="E17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>58666666666.666664</v>
       </c>
       <c r="F17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>58666666666.666664</v>
       </c>
       <c r="G17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>58666666666.666664</v>
       </c>
       <c r="H17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>58666666666.666664</v>
       </c>
       <c r="I17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>58666666666.666664</v>
       </c>
       <c r="J17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>58666666666.666664</v>
       </c>
       <c r="K17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>58666666666.666664</v>
       </c>
       <c r="L17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>58666666666.666664</v>
       </c>
       <c r="M17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>58666666666.666664</v>
       </c>
       <c r="N17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>58666666666.666664</v>
       </c>
       <c r="O17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>58666666666.666664</v>
       </c>
       <c r="P17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>58666666666.666664</v>
       </c>
       <c r="Q17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>58666666666.666664</v>
       </c>
       <c r="R17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>58666666666.666664</v>
       </c>
       <c r="S17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>58666666666.666664</v>
       </c>
       <c r="T17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>58666666666.666664</v>
       </c>
       <c r="U17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>58666666666.666664</v>
       </c>
       <c r="V17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>58666666666.666664</v>
       </c>
       <c r="W17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>58666666666.666664</v>
       </c>
       <c r="X17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>58666666666.666664</v>
       </c>
       <c r="Y17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>58666666666.666664</v>
       </c>
       <c r="Z17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>58666666666.666664</v>
       </c>
       <c r="AA17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>58666666666.666664</v>
       </c>
       <c r="AB17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>58666666666.666664</v>
       </c>
       <c r="AC17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>58666666666.666664</v>
       </c>
       <c r="AD17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>58666666666.666664</v>
       </c>
       <c r="AE17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>58666666666.666664</v>
       </c>
       <c r="AF17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>58666666666.666664</v>
       </c>
       <c r="AG17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>58666666666.666664</v>
       </c>
       <c r="AH17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>58666666666.666664</v>
       </c>
       <c r="AI17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>58666666666.666664</v>
       </c>
     </row>
@@ -22115,131 +22127,131 @@
         <v>0</v>
       </c>
       <c r="D18">
-        <f t="shared" ref="D18:AI18" si="9">C18</f>
+        <f t="shared" ref="D18:AI18" si="8">C18</f>
         <v>0</v>
       </c>
       <c r="E18">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="F18">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="G18">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="H18">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="I18">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="J18">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="K18">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="L18">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="M18">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="N18">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="O18">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="P18">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="Q18">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="R18">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="S18">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="T18">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="U18">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="V18">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="W18">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="X18">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="Y18">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="Z18">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AA18">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AB18">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AC18">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AD18">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AE18">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AF18">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AG18">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AH18">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AI18">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
@@ -22256,131 +22268,131 @@
         <v>105596954960000</v>
       </c>
       <c r="D19">
-        <f t="shared" ref="D19:AI19" si="10">C19</f>
+        <f t="shared" ref="D19:AI19" si="9">C19</f>
         <v>105596954960000</v>
       </c>
       <c r="E19">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>105596954960000</v>
       </c>
       <c r="F19">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>105596954960000</v>
       </c>
       <c r="G19">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>105596954960000</v>
       </c>
       <c r="H19">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>105596954960000</v>
       </c>
       <c r="I19">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>105596954960000</v>
       </c>
       <c r="J19">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>105596954960000</v>
       </c>
       <c r="K19">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>105596954960000</v>
       </c>
       <c r="L19">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>105596954960000</v>
       </c>
       <c r="M19">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>105596954960000</v>
       </c>
       <c r="N19">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>105596954960000</v>
       </c>
       <c r="O19">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>105596954960000</v>
       </c>
       <c r="P19">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>105596954960000</v>
       </c>
       <c r="Q19">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>105596954960000</v>
       </c>
       <c r="R19">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>105596954960000</v>
       </c>
       <c r="S19">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>105596954960000</v>
       </c>
       <c r="T19">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>105596954960000</v>
       </c>
       <c r="U19">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>105596954960000</v>
       </c>
       <c r="V19">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>105596954960000</v>
       </c>
       <c r="W19">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>105596954960000</v>
       </c>
       <c r="X19">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>105596954960000</v>
       </c>
       <c r="Y19">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>105596954960000</v>
       </c>
       <c r="Z19">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>105596954960000</v>
       </c>
       <c r="AA19">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>105596954960000</v>
       </c>
       <c r="AB19">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>105596954960000</v>
       </c>
       <c r="AC19">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>105596954960000</v>
       </c>
       <c r="AD19">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>105596954960000</v>
       </c>
       <c r="AE19">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>105596954960000</v>
       </c>
       <c r="AF19">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>105596954960000</v>
       </c>
       <c r="AG19">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>105596954960000</v>
       </c>
       <c r="AH19">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>105596954960000</v>
       </c>
       <c r="AI19">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>105596954960000</v>
       </c>
     </row>
@@ -22397,131 +22409,131 @@
         <v>16087533489000</v>
       </c>
       <c r="D20" s="31">
-        <f t="shared" ref="D20:AI20" si="11">C20</f>
+        <f t="shared" ref="D20:AI20" si="10">C20</f>
         <v>16087533489000</v>
       </c>
       <c r="E20" s="31">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>16087533489000</v>
       </c>
       <c r="F20" s="31">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>16087533489000</v>
       </c>
       <c r="G20" s="31">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>16087533489000</v>
       </c>
       <c r="H20" s="31">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>16087533489000</v>
       </c>
       <c r="I20" s="31">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>16087533489000</v>
       </c>
       <c r="J20" s="31">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>16087533489000</v>
       </c>
       <c r="K20" s="31">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>16087533489000</v>
       </c>
       <c r="L20" s="31">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>16087533489000</v>
       </c>
       <c r="M20" s="31">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>16087533489000</v>
       </c>
       <c r="N20" s="31">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>16087533489000</v>
       </c>
       <c r="O20" s="31">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>16087533489000</v>
       </c>
       <c r="P20" s="31">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>16087533489000</v>
       </c>
       <c r="Q20" s="31">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>16087533489000</v>
       </c>
       <c r="R20" s="31">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>16087533489000</v>
       </c>
       <c r="S20" s="31">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>16087533489000</v>
       </c>
       <c r="T20" s="31">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>16087533489000</v>
       </c>
       <c r="U20" s="31">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>16087533489000</v>
       </c>
       <c r="V20" s="31">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>16087533489000</v>
       </c>
       <c r="W20" s="31">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>16087533489000</v>
       </c>
       <c r="X20" s="31">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>16087533489000</v>
       </c>
       <c r="Y20" s="31">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>16087533489000</v>
       </c>
       <c r="Z20" s="31">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>16087533489000</v>
       </c>
       <c r="AA20" s="31">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>16087533489000</v>
       </c>
       <c r="AB20" s="31">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>16087533489000</v>
       </c>
       <c r="AC20" s="31">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>16087533489000</v>
       </c>
       <c r="AD20" s="31">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>16087533489000</v>
       </c>
       <c r="AE20" s="31">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>16087533489000</v>
       </c>
       <c r="AF20" s="31">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>16087533489000</v>
       </c>
       <c r="AG20" s="31">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>16087533489000</v>
       </c>
       <c r="AH20" s="31">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>16087533489000</v>
       </c>
       <c r="AI20" s="31">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>16087533489000</v>
       </c>
     </row>
@@ -23630,7 +23642,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A1" s="94"/>
+      <c r="A1" s="93"/>
       <c r="B1" s="95" t="s">
         <v>559</v>
       </c>
@@ -23640,22 +23652,22 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A2" s="94"/>
-      <c r="B2" s="94" t="s">
+      <c r="A2" s="93"/>
+      <c r="B2" s="93" t="s">
         <v>561</v>
       </c>
-      <c r="C2" s="94" t="s">
+      <c r="C2" s="93" t="s">
         <v>562</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A3" s="94" t="s">
+      <c r="A3" s="93" t="s">
         <v>563</v>
       </c>
-      <c r="B3" s="94">
+      <c r="B3" s="93">
         <v>942.63</v>
       </c>
-      <c r="C3" s="94">
+      <c r="C3" s="93">
         <v>14262</v>
       </c>
     </row>
@@ -23686,7 +23698,7 @@
       <c r="A9" s="85" t="s">
         <v>567</v>
       </c>
-      <c r="B9" s="96">
+      <c r="B9" s="94">
         <f>(C3*B6)/(B3*B7)</f>
         <v>3616.0720537220332</v>
       </c>
@@ -23708,8 +23720,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14:XFD14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -27441,10 +27453,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L25"/>
+  <dimension ref="A1:AG34"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="X37" sqref="X37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -27453,6 +27465,7 @@
     <col min="2" max="2" width="16.86328125" customWidth="1"/>
     <col min="3" max="3" width="15.59765625" customWidth="1"/>
     <col min="4" max="4" width="22.73046875" customWidth="1"/>
+    <col min="6" max="6" width="11.59765625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15.1328125" customWidth="1"/>
     <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11" bestFit="1" customWidth="1"/>
@@ -27818,7 +27831,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A17" s="55" t="s">
         <v>290</v>
       </c>
@@ -27835,7 +27848,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>267</v>
       </c>
@@ -27864,7 +27877,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A19" s="55" t="s">
         <v>268</v>
       </c>
@@ -27896,7 +27909,7 @@
         <v>6.7451599347432651E-3</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>269</v>
       </c>
@@ -27928,7 +27941,7 @@
         <v>0.13833916247672218</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>169</v>
       </c>
@@ -27960,7 +27973,7 @@
         <v>4.4274552734519634E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A22" s="53" t="s">
         <v>285</v>
       </c>
@@ -27980,7 +27993,7 @@
         <v>0.25979518811534769</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A23" s="53" t="s">
         <v>286</v>
       </c>
@@ -28000,7 +28013,7 @@
         <v>0.55084593673866733</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:33" x14ac:dyDescent="0.45">
       <c r="I24" t="s">
         <v>10</v>
       </c>
@@ -28016,7 +28029,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:33" x14ac:dyDescent="0.45">
       <c r="I25" t="s">
         <v>523</v>
       </c>
@@ -28032,6 +28045,510 @@
         <f>SUM(D5,D13,D21,L6,L13)</f>
         <v>2385048485823980</v>
       </c>
+    </row>
+    <row r="28" spans="1:33" x14ac:dyDescent="0.45">
+      <c r="A28" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="29" spans="1:33" x14ac:dyDescent="0.45">
+      <c r="B29">
+        <v>2019</v>
+      </c>
+      <c r="C29">
+        <v>2020</v>
+      </c>
+      <c r="D29">
+        <v>2021</v>
+      </c>
+      <c r="E29">
+        <v>2022</v>
+      </c>
+      <c r="F29">
+        <v>2023</v>
+      </c>
+      <c r="G29">
+        <v>2024</v>
+      </c>
+      <c r="H29">
+        <v>2025</v>
+      </c>
+      <c r="I29">
+        <v>2026</v>
+      </c>
+      <c r="J29">
+        <v>2027</v>
+      </c>
+      <c r="K29">
+        <v>2028</v>
+      </c>
+      <c r="L29">
+        <v>2029</v>
+      </c>
+      <c r="M29">
+        <v>2030</v>
+      </c>
+      <c r="N29">
+        <v>2031</v>
+      </c>
+      <c r="O29">
+        <v>2032</v>
+      </c>
+      <c r="P29">
+        <v>2033</v>
+      </c>
+      <c r="Q29">
+        <v>2034</v>
+      </c>
+      <c r="R29">
+        <v>2035</v>
+      </c>
+      <c r="S29">
+        <v>2036</v>
+      </c>
+      <c r="T29">
+        <v>2037</v>
+      </c>
+      <c r="U29">
+        <v>2038</v>
+      </c>
+      <c r="V29">
+        <v>2039</v>
+      </c>
+      <c r="W29">
+        <v>2040</v>
+      </c>
+      <c r="X29">
+        <v>2041</v>
+      </c>
+      <c r="Y29">
+        <v>2042</v>
+      </c>
+      <c r="Z29">
+        <v>2043</v>
+      </c>
+      <c r="AA29">
+        <v>2044</v>
+      </c>
+      <c r="AB29">
+        <v>2045</v>
+      </c>
+      <c r="AC29">
+        <v>2046</v>
+      </c>
+      <c r="AD29">
+        <v>2047</v>
+      </c>
+      <c r="AE29">
+        <v>2048</v>
+      </c>
+      <c r="AF29">
+        <v>2049</v>
+      </c>
+      <c r="AG29">
+        <v>2050</v>
+      </c>
+    </row>
+    <row r="30" spans="1:33" x14ac:dyDescent="0.45">
+      <c r="A30" t="s">
+        <v>569</v>
+      </c>
+      <c r="B30">
+        <f>$B$13</f>
+        <v>670364225570218.5</v>
+      </c>
+      <c r="C30">
+        <f t="shared" ref="C30:AG30" si="6">$B$13</f>
+        <v>670364225570218.5</v>
+      </c>
+      <c r="D30">
+        <f t="shared" si="6"/>
+        <v>670364225570218.5</v>
+      </c>
+      <c r="E30">
+        <f t="shared" si="6"/>
+        <v>670364225570218.5</v>
+      </c>
+      <c r="F30">
+        <f t="shared" si="6"/>
+        <v>670364225570218.5</v>
+      </c>
+      <c r="G30">
+        <f t="shared" si="6"/>
+        <v>670364225570218.5</v>
+      </c>
+      <c r="H30">
+        <f t="shared" si="6"/>
+        <v>670364225570218.5</v>
+      </c>
+      <c r="I30">
+        <f t="shared" si="6"/>
+        <v>670364225570218.5</v>
+      </c>
+      <c r="J30">
+        <f t="shared" si="6"/>
+        <v>670364225570218.5</v>
+      </c>
+      <c r="K30">
+        <f t="shared" si="6"/>
+        <v>670364225570218.5</v>
+      </c>
+      <c r="L30">
+        <f t="shared" si="6"/>
+        <v>670364225570218.5</v>
+      </c>
+      <c r="M30">
+        <f t="shared" si="6"/>
+        <v>670364225570218.5</v>
+      </c>
+      <c r="N30">
+        <f t="shared" si="6"/>
+        <v>670364225570218.5</v>
+      </c>
+      <c r="O30">
+        <f t="shared" si="6"/>
+        <v>670364225570218.5</v>
+      </c>
+      <c r="P30">
+        <f t="shared" si="6"/>
+        <v>670364225570218.5</v>
+      </c>
+      <c r="Q30">
+        <f t="shared" si="6"/>
+        <v>670364225570218.5</v>
+      </c>
+      <c r="R30">
+        <f t="shared" si="6"/>
+        <v>670364225570218.5</v>
+      </c>
+      <c r="S30">
+        <f t="shared" si="6"/>
+        <v>670364225570218.5</v>
+      </c>
+      <c r="T30">
+        <f t="shared" si="6"/>
+        <v>670364225570218.5</v>
+      </c>
+      <c r="U30">
+        <f t="shared" si="6"/>
+        <v>670364225570218.5</v>
+      </c>
+      <c r="V30">
+        <f t="shared" si="6"/>
+        <v>670364225570218.5</v>
+      </c>
+      <c r="W30">
+        <f t="shared" si="6"/>
+        <v>670364225570218.5</v>
+      </c>
+      <c r="X30">
+        <f t="shared" si="6"/>
+        <v>670364225570218.5</v>
+      </c>
+      <c r="Y30">
+        <f t="shared" si="6"/>
+        <v>670364225570218.5</v>
+      </c>
+      <c r="Z30">
+        <f t="shared" si="6"/>
+        <v>670364225570218.5</v>
+      </c>
+      <c r="AA30">
+        <f t="shared" si="6"/>
+        <v>670364225570218.5</v>
+      </c>
+      <c r="AB30">
+        <f t="shared" si="6"/>
+        <v>670364225570218.5</v>
+      </c>
+      <c r="AC30">
+        <f t="shared" si="6"/>
+        <v>670364225570218.5</v>
+      </c>
+      <c r="AD30">
+        <f t="shared" si="6"/>
+        <v>670364225570218.5</v>
+      </c>
+      <c r="AE30">
+        <f t="shared" si="6"/>
+        <v>670364225570218.5</v>
+      </c>
+      <c r="AF30">
+        <f t="shared" si="6"/>
+        <v>670364225570218.5</v>
+      </c>
+      <c r="AG30">
+        <f t="shared" si="6"/>
+        <v>670364225570218.5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:33" x14ac:dyDescent="0.45">
+      <c r="A31" t="s">
+        <v>570</v>
+      </c>
+      <c r="B31">
+        <v>0</v>
+      </c>
+      <c r="C31">
+        <v>0</v>
+      </c>
+      <c r="D31">
+        <v>0</v>
+      </c>
+      <c r="E31">
+        <v>0</v>
+      </c>
+      <c r="F31">
+        <v>0</v>
+      </c>
+      <c r="G31">
+        <v>0</v>
+      </c>
+      <c r="H31">
+        <v>0</v>
+      </c>
+      <c r="I31">
+        <v>0</v>
+      </c>
+      <c r="J31">
+        <v>0</v>
+      </c>
+      <c r="K31">
+        <v>0</v>
+      </c>
+      <c r="L31">
+        <v>0</v>
+      </c>
+      <c r="M31">
+        <v>0</v>
+      </c>
+      <c r="N31">
+        <v>0</v>
+      </c>
+      <c r="O31">
+        <v>0</v>
+      </c>
+      <c r="P31">
+        <v>0</v>
+      </c>
+      <c r="Q31">
+        <v>0</v>
+      </c>
+      <c r="R31">
+        <v>0</v>
+      </c>
+      <c r="S31">
+        <v>0</v>
+      </c>
+      <c r="T31">
+        <v>0</v>
+      </c>
+      <c r="U31">
+        <v>0</v>
+      </c>
+      <c r="V31">
+        <v>0</v>
+      </c>
+      <c r="W31">
+        <v>0</v>
+      </c>
+      <c r="X31">
+        <v>0</v>
+      </c>
+      <c r="Y31" s="31">
+        <f>'BAU Total Primary Fuel Use'!Y14-'Petroleum Products'!Y30</f>
+        <v>663774429781.5</v>
+      </c>
+      <c r="Z31" s="31">
+        <f>'BAU Total Primary Fuel Use'!Z14-'Petroleum Products'!Z30</f>
+        <v>44874774429781.5</v>
+      </c>
+      <c r="AA31" s="31">
+        <f>'BAU Total Primary Fuel Use'!AA14-'Petroleum Products'!AA30</f>
+        <v>88899774429781.5</v>
+      </c>
+      <c r="AB31" s="31">
+        <f>'BAU Total Primary Fuel Use'!AB14-'Petroleum Products'!AB30</f>
+        <v>132672774429781.5</v>
+      </c>
+      <c r="AC31" s="31">
+        <f>'BAU Total Primary Fuel Use'!AC14-'Petroleum Products'!AC30</f>
+        <v>185451774429781.5</v>
+      </c>
+      <c r="AD31" s="31">
+        <f>'BAU Total Primary Fuel Use'!AD14-'Petroleum Products'!AD30</f>
+        <v>238134774429781.5</v>
+      </c>
+      <c r="AE31" s="31">
+        <f>'BAU Total Primary Fuel Use'!AE14-'Petroleum Products'!AE30</f>
+        <v>290792774429781.5</v>
+      </c>
+      <c r="AF31" s="31">
+        <f>'BAU Total Primary Fuel Use'!AF14-'Petroleum Products'!AF30</f>
+        <v>343285774429781.5</v>
+      </c>
+      <c r="AG31" s="31">
+        <f>'BAU Total Primary Fuel Use'!AG14-'Petroleum Products'!AG30</f>
+        <v>395365774429781.5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:33" x14ac:dyDescent="0.45">
+      <c r="A32" t="s">
+        <v>571</v>
+      </c>
+      <c r="B32" s="31">
+        <f>B30-'BAU Total Primary Fuel Use'!B14</f>
+        <v>417312225570218.5</v>
+      </c>
+      <c r="C32" s="31">
+        <f>C30-'BAU Total Primary Fuel Use'!C14</f>
+        <v>479955225570218.5</v>
+      </c>
+      <c r="D32" s="31">
+        <f>D30-'BAU Total Primary Fuel Use'!D14</f>
+        <v>482175225570218.5</v>
+      </c>
+      <c r="E32" s="31">
+        <f>E30-'BAU Total Primary Fuel Use'!E14</f>
+        <v>492471225570218.5</v>
+      </c>
+      <c r="F32" s="31">
+        <f>F30-'BAU Total Primary Fuel Use'!F14</f>
+        <v>476330225570218.5</v>
+      </c>
+      <c r="G32" s="31">
+        <f>G30-'BAU Total Primary Fuel Use'!G14</f>
+        <v>462978225570218.5</v>
+      </c>
+      <c r="H32" s="31">
+        <f>H30-'BAU Total Primary Fuel Use'!H14</f>
+        <v>451019225570218.5</v>
+      </c>
+      <c r="I32" s="31">
+        <f>I30-'BAU Total Primary Fuel Use'!I14</f>
+        <v>433034225570218.5</v>
+      </c>
+      <c r="J32" s="31">
+        <f>J30-'BAU Total Primary Fuel Use'!J14</f>
+        <v>415810225570218.5</v>
+      </c>
+      <c r="K32" s="31">
+        <f>K30-'BAU Total Primary Fuel Use'!K14</f>
+        <v>399214225570218.5</v>
+      </c>
+      <c r="L32" s="31">
+        <f>L30-'BAU Total Primary Fuel Use'!L14</f>
+        <v>383130225570218.5</v>
+      </c>
+      <c r="M32" s="31">
+        <f>M30-'BAU Total Primary Fuel Use'!M14</f>
+        <v>367121225570218.5</v>
+      </c>
+      <c r="N32" s="31">
+        <f>N30-'BAU Total Primary Fuel Use'!N14</f>
+        <v>346554225570218.5</v>
+      </c>
+      <c r="O32" s="31">
+        <f>O30-'BAU Total Primary Fuel Use'!O14</f>
+        <v>326227225570218.5</v>
+      </c>
+      <c r="P32" s="31">
+        <f>P30-'BAU Total Primary Fuel Use'!P14</f>
+        <v>306106225570218.5</v>
+      </c>
+      <c r="Q32" s="31">
+        <f>Q30-'BAU Total Primary Fuel Use'!Q14</f>
+        <v>286166225570218.5</v>
+      </c>
+      <c r="R32" s="31">
+        <f>R30-'BAU Total Primary Fuel Use'!R14</f>
+        <v>266254225570218.5</v>
+      </c>
+      <c r="S32" s="31">
+        <f>S30-'BAU Total Primary Fuel Use'!S14</f>
+        <v>229978225570218.5</v>
+      </c>
+      <c r="T32" s="31">
+        <f>T30-'BAU Total Primary Fuel Use'!T14</f>
+        <v>194016225570218.5</v>
+      </c>
+      <c r="U32" s="31">
+        <f>U30-'BAU Total Primary Fuel Use'!U14</f>
+        <v>158523225570218.5</v>
+      </c>
+      <c r="V32" s="31">
+        <f>V30-'BAU Total Primary Fuel Use'!V14</f>
+        <v>123448225570218.5</v>
+      </c>
+      <c r="W32" s="31">
+        <f>W30-'BAU Total Primary Fuel Use'!W14</f>
+        <v>88784225570218.5</v>
+      </c>
+      <c r="X32" s="31">
+        <f>X30-'BAU Total Primary Fuel Use'!X14</f>
+        <v>43903225570218.5</v>
+      </c>
+      <c r="Y32" s="31">
+        <v>0</v>
+      </c>
+      <c r="Z32" s="31">
+        <v>0</v>
+      </c>
+      <c r="AA32" s="31">
+        <v>0</v>
+      </c>
+      <c r="AB32" s="31">
+        <v>0</v>
+      </c>
+      <c r="AC32" s="31">
+        <v>0</v>
+      </c>
+      <c r="AD32" s="31">
+        <v>0</v>
+      </c>
+      <c r="AE32" s="31">
+        <v>0</v>
+      </c>
+      <c r="AF32" s="31">
+        <v>0</v>
+      </c>
+      <c r="AG32" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="2:33" x14ac:dyDescent="0.45">
+      <c r="B34" s="31"/>
+      <c r="C34" s="31"/>
+      <c r="D34" s="31"/>
+      <c r="E34" s="31"/>
+      <c r="F34" s="31"/>
+      <c r="G34" s="31"/>
+      <c r="H34" s="31"/>
+      <c r="I34" s="31"/>
+      <c r="J34" s="31"/>
+      <c r="K34" s="31"/>
+      <c r="L34" s="31"/>
+      <c r="M34" s="31"/>
+      <c r="N34" s="31"/>
+      <c r="O34" s="31"/>
+      <c r="P34" s="31"/>
+      <c r="Q34" s="31"/>
+      <c r="R34" s="31"/>
+      <c r="S34" s="31"/>
+      <c r="T34" s="31"/>
+      <c r="U34" s="31"/>
+      <c r="V34" s="31"/>
+      <c r="W34" s="31"/>
+      <c r="X34" s="31"/>
+      <c r="Y34" s="31"/>
+      <c r="Z34" s="31"/>
+      <c r="AA34" s="31"/>
+      <c r="AB34" s="31"/>
+      <c r="AC34" s="31"/>
+      <c r="AD34" s="31"/>
+      <c r="AE34" s="31"/>
+      <c r="AF34" s="31"/>
+      <c r="AG34" s="31"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Fix natural gas unit conversion error
</commit_message>
<xml_diff>
--- a/InputData/fuels/BFPIaE/BAU Fuel Production Imports and Exports.xlsx
+++ b/InputData/fuels/BFPIaE/BAU Fuel Production Imports and Exports.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-india\InputData\fuels\BFPIaE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26146235-B81E-415C-B657-FD80215503E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0BF9A13-C0FB-49D3-BDB5-EB19282F97BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="684" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="684" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="4" r:id="rId1"/>
@@ -39,7 +39,7 @@
     <definedName name="preferences.energyunits">[2]Preferences!$C$3</definedName>
     <definedName name="Preferences.PowerUnits">[2]Preferences!$C$5</definedName>
   </definedNames>
-  <calcPr calcId="191029" iterate="1" iterateDelta="1.0000000000000001E-5"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -1855,14 +1855,14 @@
     <numFmt numFmtId="170" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="171" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="172" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="174" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="#,##0.0_);\(#,##0.0\);&quot;-&quot;;@"/>
-    <numFmt numFmtId="178" formatCode="#,##0.0_);\(#,##0.0\);&quot;-&quot;_);@"/>
-    <numFmt numFmtId="183" formatCode="0%;\ \(0%\);\ \-"/>
-    <numFmt numFmtId="192" formatCode="&quot;$&quot;#,##0\ ;\(&quot;$&quot;#,##0\)"/>
-    <numFmt numFmtId="193" formatCode="0.00_)"/>
-    <numFmt numFmtId="194" formatCode="mm/dd/yy"/>
-    <numFmt numFmtId="210" formatCode="0.0_ ;\-0.0\ "/>
+    <numFmt numFmtId="173" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="174" formatCode="#,##0.0_);\(#,##0.0\);&quot;-&quot;;@"/>
+    <numFmt numFmtId="175" formatCode="#,##0.0_);\(#,##0.0\);&quot;-&quot;_);@"/>
+    <numFmt numFmtId="176" formatCode="0%;\ \(0%\);\ \-"/>
+    <numFmt numFmtId="177" formatCode="&quot;$&quot;#,##0\ ;\(&quot;$&quot;#,##0\)"/>
+    <numFmt numFmtId="178" formatCode="0.00_)"/>
+    <numFmt numFmtId="179" formatCode="mm/dd/yy"/>
+    <numFmt numFmtId="180" formatCode="0.0_ ;\-0.0\ "/>
   </numFmts>
   <fonts count="91">
     <font>
@@ -3409,15 +3409,15 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0"/>
-    <xf numFmtId="183" fontId="24" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="178" fontId="22" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="176" fontId="24" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="175" fontId="22" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="25" fillId="14" borderId="25" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="177" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="174" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="32" applyNumberFormat="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
-    <xf numFmtId="183" fontId="24" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="176" fontId="24" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3770,7 +3770,7 @@
     <xf numFmtId="0" fontId="23" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
-    <xf numFmtId="178" fontId="22" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="175" fontId="22" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="23" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
@@ -3833,7 +3833,7 @@
     <xf numFmtId="0" fontId="55" fillId="0" borderId="0" applyNumberFormat="0" applyAlignment="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="192" fontId="54" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="177" fontId="54" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="3" fontId="56" fillId="0" borderId="0">
       <alignment horizontal="right"/>
     </xf>
@@ -3871,10 +3871,10 @@
     <xf numFmtId="10" fontId="6" fillId="64" borderId="21" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="10" fontId="6" fillId="64" borderId="21" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="10" fontId="6" fillId="64" borderId="21" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="193" fontId="62" fillId="0" borderId="36" applyNumberFormat="0" applyFill="0" applyBorder="0">
+    <xf numFmtId="178" fontId="62" fillId="0" borderId="36" applyNumberFormat="0" applyFill="0" applyBorder="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="193" fontId="63" fillId="0" borderId="0"/>
+    <xf numFmtId="178" fontId="63" fillId="0" borderId="0"/>
     <xf numFmtId="166" fontId="64" fillId="0" borderId="34">
       <alignment horizontal="right"/>
     </xf>
@@ -3911,7 +3911,7 @@
     <xf numFmtId="9" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="194" fontId="70" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="179" fontId="70" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="56" fillId="0" borderId="0" applyBorder="0">
@@ -3974,13 +3974,13 @@
     <xf numFmtId="0" fontId="88" fillId="45" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="174" fontId="22" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="173" fontId="22" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="23" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
-    <xf numFmtId="178" fontId="22" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="183" fontId="24" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="175" fontId="22" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="176" fontId="24" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
@@ -3992,7 +3992,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
     <xf numFmtId="171" fontId="23" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="25" fillId="14" borderId="25" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="183" fontId="24" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="176" fontId="24" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -4005,7 +4005,7 @@
     <xf numFmtId="1" fontId="90" fillId="42" borderId="33">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="210" fontId="27" fillId="42" borderId="0" applyBorder="0" applyProtection="0">
+    <xf numFmtId="180" fontId="27" fillId="42" borderId="0" applyBorder="0" applyProtection="0">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -4110,7 +4110,7 @@
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="99">
+  <cellXfs count="100">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -4266,16 +4266,17 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="175" fontId="22" fillId="8" borderId="0" xfId="22" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="175" fontId="26" fillId="6" borderId="0" xfId="24" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="15" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="178" fontId="22" fillId="8" borderId="0" xfId="22" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="26" fillId="6" borderId="0" xfId="24" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="639">
     <cellStyle name="20% - Accent1 2" xfId="187" xr:uid="{160FCEB9-CDBA-4190-9D8D-5901C18EB9A0}"/>
@@ -5684,10 +5685,10 @@
       <selection activeCell="C114" sqref="C114"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="2" max="2" width="76.28515625" customWidth="1"/>
-    <col min="4" max="4" width="78.85546875" customWidth="1"/>
+    <col min="2" max="2" width="76.26953125" customWidth="1"/>
+    <col min="4" max="4" width="78.81640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -6646,15 +6647,15 @@
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="2" max="2" width="14" customWidth="1"/>
-    <col min="6" max="6" width="10.7109375" customWidth="1"/>
-    <col min="9" max="9" width="18.85546875" customWidth="1"/>
+    <col min="6" max="6" width="10.7265625" customWidth="1"/>
+    <col min="9" max="9" width="18.81640625" customWidth="1"/>
     <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:43" ht="15.75" thickBot="1">
+    <row r="1" spans="1:43" ht="15" thickBot="1">
       <c r="A1" s="1" t="s">
         <v>357</v>
       </c>
@@ -6955,7 +6956,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="3" spans="1:43" ht="15.75" thickBot="1">
+    <row r="3" spans="1:43" ht="15" thickBot="1">
       <c r="A3" s="63" t="s">
         <v>231</v>
       </c>
@@ -8153,7 +8154,7 @@
         <v>1588548260249999.8</v>
       </c>
     </row>
-    <row r="11" spans="1:43" ht="26.25">
+    <row r="11" spans="1:43" ht="26.5">
       <c r="A11" s="53" t="s">
         <v>358</v>
       </c>
@@ -8349,12 +8350,12 @@
       <selection activeCell="R1" sqref="R1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="20.28515625" customWidth="1"/>
+    <col min="1" max="1" width="20.26953125" customWidth="1"/>
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="20" customWidth="1"/>
-    <col min="10" max="10" width="10.28515625" customWidth="1"/>
+    <col min="10" max="10" width="10.26953125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:35">
@@ -8389,7 +8390,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="2" spans="1:35" ht="30">
+    <row r="2" spans="1:35" ht="29">
       <c r="B2">
         <v>2011</v>
       </c>
@@ -9150,20 +9151,20 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.81640625" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="12" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="12" bestFit="1" customWidth="1"/>
     <col min="12" max="13" width="12" bestFit="1" customWidth="1"/>
     <col min="17" max="18" width="12" bestFit="1" customWidth="1"/>
     <col min="22" max="23" width="12" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="12.42578125" customWidth="1"/>
+    <col min="27" max="27" width="12.453125" customWidth="1"/>
     <col min="28" max="28" width="12" bestFit="1" customWidth="1"/>
     <col min="32" max="33" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" ht="30">
+    <row r="1" spans="1:35" ht="29">
       <c r="A1" s="61" t="s">
         <v>482</v>
       </c>
@@ -9757,11 +9758,11 @@
       <selection pane="bottomRight" activeCell="F70" sqref="F70"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="20.85546875" style="7" hidden="1" customWidth="1"/>
-    <col min="2" max="2" width="45.7109375" style="7" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="7"/>
+    <col min="1" max="1" width="20.81640625" style="7" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="45.7265625" style="7" customWidth="1"/>
+    <col min="3" max="16384" width="9.1796875" style="7"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:37" ht="15" customHeight="1" thickBot="1">
@@ -16393,44 +16394,44 @@
     </row>
     <row r="77" spans="1:37" ht="15" customHeight="1" thickBot="1"/>
     <row r="78" spans="1:37" ht="15" customHeight="1">
-      <c r="B78" s="96" t="s">
+      <c r="B78" s="98" t="s">
         <v>164</v>
       </c>
-      <c r="C78" s="96"/>
-      <c r="D78" s="96"/>
-      <c r="E78" s="96"/>
-      <c r="F78" s="96"/>
-      <c r="G78" s="96"/>
-      <c r="H78" s="96"/>
-      <c r="I78" s="96"/>
-      <c r="J78" s="96"/>
-      <c r="K78" s="96"/>
-      <c r="L78" s="96"/>
-      <c r="M78" s="96"/>
-      <c r="N78" s="96"/>
-      <c r="O78" s="96"/>
-      <c r="P78" s="96"/>
-      <c r="Q78" s="96"/>
-      <c r="R78" s="96"/>
-      <c r="S78" s="96"/>
-      <c r="T78" s="96"/>
-      <c r="U78" s="96"/>
-      <c r="V78" s="96"/>
-      <c r="W78" s="96"/>
-      <c r="X78" s="96"/>
-      <c r="Y78" s="96"/>
-      <c r="Z78" s="96"/>
-      <c r="AA78" s="96"/>
-      <c r="AB78" s="96"/>
-      <c r="AC78" s="96"/>
-      <c r="AD78" s="96"/>
-      <c r="AE78" s="96"/>
-      <c r="AF78" s="96"/>
-      <c r="AG78" s="96"/>
-      <c r="AH78" s="96"/>
-      <c r="AI78" s="96"/>
-      <c r="AJ78" s="96"/>
-      <c r="AK78" s="96"/>
+      <c r="C78" s="98"/>
+      <c r="D78" s="98"/>
+      <c r="E78" s="98"/>
+      <c r="F78" s="98"/>
+      <c r="G78" s="98"/>
+      <c r="H78" s="98"/>
+      <c r="I78" s="98"/>
+      <c r="J78" s="98"/>
+      <c r="K78" s="98"/>
+      <c r="L78" s="98"/>
+      <c r="M78" s="98"/>
+      <c r="N78" s="98"/>
+      <c r="O78" s="98"/>
+      <c r="P78" s="98"/>
+      <c r="Q78" s="98"/>
+      <c r="R78" s="98"/>
+      <c r="S78" s="98"/>
+      <c r="T78" s="98"/>
+      <c r="U78" s="98"/>
+      <c r="V78" s="98"/>
+      <c r="W78" s="98"/>
+      <c r="X78" s="98"/>
+      <c r="Y78" s="98"/>
+      <c r="Z78" s="98"/>
+      <c r="AA78" s="98"/>
+      <c r="AB78" s="98"/>
+      <c r="AC78" s="98"/>
+      <c r="AD78" s="98"/>
+      <c r="AE78" s="98"/>
+      <c r="AF78" s="98"/>
+      <c r="AG78" s="98"/>
+      <c r="AH78" s="98"/>
+      <c r="AI78" s="98"/>
+      <c r="AJ78" s="98"/>
+      <c r="AK78" s="98"/>
     </row>
     <row r="79" spans="1:37" ht="15" customHeight="1">
       <c r="B79" s="11" t="s">
@@ -16484,12 +16485,12 @@
   <dimension ref="A1:AI23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="36.28515625" customWidth="1"/>
+    <col min="1" max="1" width="36.26953125" customWidth="1"/>
     <col min="2" max="35" width="13" customWidth="1"/>
   </cols>
   <sheetData>
@@ -16852,141 +16853,141 @@
       <c r="A4" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="12">
+      <c r="B4" s="99">
         <f>'Natural Gas'!B14</f>
-        <v>1175328000</v>
+        <v>1175328000000000</v>
       </c>
       <c r="C4" s="12">
         <f>'Natural Gas'!C14</f>
-        <v>1214506491.7213566</v>
+        <v>1214506491721356.5</v>
       </c>
       <c r="D4" s="12">
         <f>'Natural Gas'!D14</f>
-        <v>1254990962.8914802</v>
+        <v>1254990962891480</v>
       </c>
       <c r="E4" s="12">
         <f>'Natural Gas'!E14</f>
-        <v>1296824947.1495094</v>
+        <v>1296824947149509.3</v>
       </c>
       <c r="F4" s="12">
         <f>'Natural Gas'!F14</f>
-        <v>1340053429.2889171</v>
+        <v>1340053429288916.8</v>
       </c>
       <c r="G4" s="12">
         <f>'Natural Gas'!G14</f>
-        <v>1384722893.6304212</v>
+        <v>1384722893630420.8</v>
       </c>
       <c r="H4" s="12">
         <f>'Natural Gas'!H14</f>
-        <v>1449342887.8482506</v>
+        <v>1449342887848250.3</v>
       </c>
       <c r="I4" s="12">
         <f>'Natural Gas'!I14</f>
-        <v>1516978462.7804024</v>
+        <v>1516978462780402</v>
       </c>
       <c r="J4" s="12">
         <f>'Natural Gas'!J14</f>
-        <v>1587770344.6394777</v>
+        <v>1587770344639477.3</v>
       </c>
       <c r="K4" s="12">
         <f>'Natural Gas'!K14</f>
-        <v>1661865826.8199208</v>
+        <v>1661865826819920.3</v>
       </c>
       <c r="L4" s="12">
         <f>'Natural Gas'!L14</f>
-        <v>1739419076.3645723</v>
+        <v>1739419076364571.8</v>
       </c>
       <c r="M4" s="12">
         <f>'Natural Gas'!M14</f>
-        <v>1816809204.9845138</v>
+        <v>1816809204984513.3</v>
       </c>
       <c r="N4" s="12">
         <f>'Natural Gas'!N14</f>
-        <v>1897642570.5386672</v>
+        <v>1897642570538666.5</v>
       </c>
       <c r="O4" s="12">
         <f>'Natural Gas'!O14</f>
-        <v>1982072369.3170054</v>
+        <v>1982072369317004.8</v>
       </c>
       <c r="P4" s="12">
         <f>'Natural Gas'!P14</f>
-        <v>2070258613.6095941</v>
+        <v>2070258613609593.5</v>
       </c>
       <c r="Q4" s="12">
         <f>'Natural Gas'!Q14</f>
-        <v>2162368434.9636559</v>
+        <v>2162368434963655.5</v>
       </c>
       <c r="R4" s="12">
         <f>'Natural Gas'!R14</f>
-        <v>2254335327.7793608</v>
+        <v>2254335327779360.5</v>
       </c>
       <c r="S4" s="12">
         <f>'Natural Gas'!S14</f>
-        <v>2350213630.5275354</v>
+        <v>2350213630527535</v>
       </c>
       <c r="T4" s="12">
         <f>'Natural Gas'!T14</f>
-        <v>2450169697.9385767</v>
+        <v>2450169697938576</v>
       </c>
       <c r="U4" s="12">
         <f>'Natural Gas'!U14</f>
-        <v>2554376959.9144449</v>
+        <v>2554376959914444</v>
       </c>
       <c r="V4" s="12">
         <f>'Natural Gas'!V14</f>
-        <v>2663016222.4401703</v>
+        <v>2663016222440169</v>
       </c>
       <c r="W4" s="12">
         <f>'Natural Gas'!W14</f>
-        <v>2782500363.6382184</v>
+        <v>2782500363638217</v>
       </c>
       <c r="X4" s="12">
         <f>'Natural Gas'!X14</f>
-        <v>2907345516.1127028</v>
+        <v>2907345516112701.5</v>
       </c>
       <c r="Y4" s="12">
         <f>'Natural Gas'!Y14</f>
-        <v>3037792217.5753059</v>
+        <v>3037792217575304.5</v>
       </c>
       <c r="Z4" s="12">
         <f>'Natural Gas'!Z14</f>
-        <v>3174091798.1773744</v>
+        <v>3174091798177372.5</v>
       </c>
       <c r="AA4" s="12">
         <f>'Natural Gas'!AA14</f>
-        <v>3316506864.7448153</v>
+        <v>3316506864744813</v>
       </c>
       <c r="AB4" s="12">
         <f>'Natural Gas'!AB14</f>
-        <v>3474467101.4868736</v>
+        <v>3474467101486871.5</v>
       </c>
       <c r="AC4" s="12">
         <f>'Natural Gas'!AC14</f>
-        <v>3639950746.866148</v>
+        <v>3639950746866146</v>
       </c>
       <c r="AD4" s="12">
         <f>'Natural Gas'!AD14</f>
-        <v>3813316129.5271754</v>
+        <v>3813316129527173.5</v>
       </c>
       <c r="AE4" s="12">
         <f>'Natural Gas'!AE14</f>
-        <v>3994938644.7692084</v>
+        <v>3994938644769206.5</v>
       </c>
       <c r="AF4" s="12">
         <f>'Natural Gas'!AF14</f>
-        <v>4185211567.4053259</v>
+        <v>4185211567405324</v>
       </c>
       <c r="AG4" s="12">
         <f>'Natural Gas'!AG14</f>
-        <v>4185211567.4053259</v>
+        <v>4185211567405324</v>
       </c>
       <c r="AH4" s="12">
         <f>'Natural Gas'!AH14</f>
-        <v>4185211567.4053259</v>
+        <v>4185211567405324</v>
       </c>
       <c r="AI4" s="12">
         <f>'Natural Gas'!AI14</f>
-        <v>4185211567.4053259</v>
+        <v>4185211567405324</v>
       </c>
     </row>
     <row r="5" spans="1:35">
@@ -19343,9 +19344,9 @@
       <selection activeCell="X33" sqref="X33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="36.28515625" customWidth="1"/>
+    <col min="1" max="1" width="36.26953125" customWidth="1"/>
     <col min="2" max="2" width="12" style="12" bestFit="1" customWidth="1"/>
     <col min="3" max="35" width="13" customWidth="1"/>
   </cols>
@@ -19744,139 +19745,139 @@
       </c>
       <c r="B4" s="12">
         <f>'Natural Gas'!B15</f>
-        <v>944568000</v>
+        <v>944568000000000</v>
       </c>
       <c r="C4" s="12">
         <f>'Natural Gas'!C15</f>
-        <v>978485825.88333893</v>
+        <v>978485825883339</v>
       </c>
       <c r="D4" s="12">
         <f>'Natural Gas'!D15</f>
-        <v>1013621583.0460061</v>
+        <v>1013621583046006.1</v>
       </c>
       <c r="E4" s="12">
         <f>'Natural Gas'!E15</f>
-        <v>1050019005.323014</v>
+        <v>1050019005323014</v>
       </c>
       <c r="F4" s="12">
         <f>'Natural Gas'!F15</f>
-        <v>1087723396.9568009</v>
+        <v>1087723396956800.9</v>
       </c>
       <c r="G4" s="12">
         <f>'Natural Gas'!G15</f>
-        <v>1126781688.9878826</v>
+        <v>1126781688987882.5</v>
       </c>
       <c r="H4" s="12">
         <f>'Natural Gas'!H15</f>
-        <v>1138906138.2336495</v>
+        <v>1138906138233649.5</v>
       </c>
       <c r="I4" s="12">
         <f>'Natural Gas'!I15</f>
-        <v>1151161049.5475791</v>
+        <v>1151161049547579</v>
       </c>
       <c r="J4" s="12">
         <f>'Natural Gas'!J15</f>
-        <v>1163547826.7337439</v>
+        <v>1163547826733743.8</v>
       </c>
       <c r="K4" s="12">
         <f>'Natural Gas'!K15</f>
-        <v>1176067888.7014952</v>
+        <v>1176067888701495</v>
       </c>
       <c r="L4" s="12">
         <f>'Natural Gas'!L15</f>
-        <v>1188722669.6279988</v>
+        <v>1188722669627998.8</v>
       </c>
       <c r="M4" s="12">
         <f>'Natural Gas'!M15</f>
-        <v>1205496447.1504569</v>
+        <v>1205496447150456.8</v>
       </c>
       <c r="N4" s="12">
         <f>'Natural Gas'!N15</f>
-        <v>1222506915.3826673</v>
+        <v>1222506915382667</v>
       </c>
       <c r="O4" s="12">
         <f>'Natural Gas'!O15</f>
-        <v>1239757414.2098768</v>
+        <v>1239757414209876.5</v>
       </c>
       <c r="P4" s="12">
         <f>'Natural Gas'!P15</f>
-        <v>1257251330.6456439</v>
+        <v>1257251330645643.8</v>
       </c>
       <c r="Q4" s="12">
         <f>'Natural Gas'!Q15</f>
-        <v>1274992099.4968545</v>
+        <v>1274992099496854.3</v>
       </c>
       <c r="R4" s="12">
         <f>'Natural Gas'!R15</f>
-        <v>1274379003.3355594</v>
+        <v>1274379003335559</v>
       </c>
       <c r="S4" s="12">
         <f>'Natural Gas'!S15</f>
-        <v>1273766201.9893482</v>
+        <v>1273766201989347.8</v>
       </c>
       <c r="T4" s="12">
         <f>'Natural Gas'!T15</f>
-        <v>1273153695.3164556</v>
+        <v>1273153695316455</v>
       </c>
       <c r="U4" s="12">
         <f>'Natural Gas'!U15</f>
-        <v>1272541483.175184</v>
+        <v>1272541483175183.5</v>
       </c>
       <c r="V4" s="12">
         <f>'Natural Gas'!V15</f>
-        <v>1271929565.4239042</v>
+        <v>1271929565423903.8</v>
       </c>
       <c r="W4" s="12">
         <f>'Natural Gas'!W15</f>
-        <v>1260606340.2859473</v>
+        <v>1260606340285946.8</v>
       </c>
       <c r="X4" s="12">
         <f>'Natural Gas'!X15</f>
-        <v>1249383919.0218921</v>
+        <v>1249383919021891.5</v>
       </c>
       <c r="Y4" s="12">
         <f>'Natural Gas'!Y15</f>
-        <v>1238261404.2353811</v>
+        <v>1238261404235380.5</v>
       </c>
       <c r="Z4" s="12">
         <f>'Natural Gas'!Z15</f>
-        <v>1227237906.5190377</v>
+        <v>1227237906519037.3</v>
       </c>
       <c r="AA4" s="12">
         <f>'Natural Gas'!AA15</f>
-        <v>1216312544.3833454</v>
+        <v>1216312544383344.8</v>
       </c>
       <c r="AB4" s="12">
         <f>'Natural Gas'!AB15</f>
-        <v>1167620883.0635505</v>
+        <v>1167620883063550</v>
       </c>
       <c r="AC4" s="12">
         <f>'Natural Gas'!AC15</f>
-        <v>1120878455.8390791</v>
+        <v>1120878455839078.6</v>
       </c>
       <c r="AD4" s="12">
         <f>'Natural Gas'!AD15</f>
-        <v>1076007230.5899463</v>
+        <v>1076007230589945.8</v>
       </c>
       <c r="AE4" s="12">
         <f>'Natural Gas'!AE15</f>
-        <v>1032932298.9932337</v>
+        <v>1032932298993233.3</v>
       </c>
       <c r="AF4" s="12">
         <f>'Natural Gas'!AF15</f>
-        <v>991581751.47063565</v>
+        <v>991581751470635.25</v>
       </c>
       <c r="AG4" s="12">
         <f>'Natural Gas'!AG15</f>
-        <v>991581751.47063565</v>
+        <v>991581751470635.25</v>
       </c>
       <c r="AH4" s="12">
         <f>'Natural Gas'!AH15</f>
-        <v>991581751.47063565</v>
+        <v>991581751470635.25</v>
       </c>
       <c r="AI4" s="12">
         <f>'Natural Gas'!AI15</f>
-        <v>991581751.47063565</v>
+        <v>991581751470635.25</v>
       </c>
     </row>
     <row r="5" spans="1:35">
@@ -22427,9 +22428,9 @@
       <selection activeCell="AE27" sqref="AE27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="36.28515625" customWidth="1"/>
+    <col min="1" max="1" width="36.26953125" customWidth="1"/>
     <col min="2" max="2" width="12" style="12" bestFit="1" customWidth="1"/>
     <col min="3" max="35" width="13" customWidth="1"/>
   </cols>
@@ -25213,15 +25214,15 @@
       <selection activeCell="B63" sqref="B63"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="26" customWidth="1"/>
-    <col min="2" max="2" width="21.28515625" customWidth="1"/>
-    <col min="3" max="3" width="26.5703125" customWidth="1"/>
-    <col min="6" max="6" width="21.140625" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" customWidth="1"/>
-    <col min="8" max="8" width="26.7109375" customWidth="1"/>
-    <col min="9" max="9" width="15.42578125" customWidth="1"/>
+    <col min="2" max="2" width="21.26953125" customWidth="1"/>
+    <col min="3" max="3" width="26.54296875" customWidth="1"/>
+    <col min="6" max="6" width="21.1796875" customWidth="1"/>
+    <col min="7" max="7" width="11.7265625" customWidth="1"/>
+    <col min="8" max="8" width="26.7265625" customWidth="1"/>
+    <col min="9" max="9" width="15.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -25592,7 +25593,7 @@
       </c>
       <c r="C25" s="38"/>
     </row>
-    <row r="26" spans="1:3" ht="30">
+    <row r="26" spans="1:3" ht="29">
       <c r="A26" s="42" t="s">
         <v>209</v>
       </c>
@@ -26076,19 +26077,19 @@
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="25.140625" customWidth="1"/>
-    <col min="2" max="2" width="22.85546875" customWidth="1"/>
-    <col min="3" max="3" width="20.7109375" customWidth="1"/>
+    <col min="1" max="1" width="25.1796875" customWidth="1"/>
+    <col min="2" max="2" width="22.81640625" customWidth="1"/>
+    <col min="3" max="3" width="20.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="93"/>
-      <c r="B1" s="95" t="s">
+      <c r="B1" s="97" t="s">
         <v>559</v>
       </c>
-      <c r="C1" s="95"/>
+      <c r="C1" s="97"/>
       <c r="D1" s="4" t="s">
         <v>560</v>
       </c>
@@ -26166,9 +26167,9 @@
       <selection activeCell="B18" sqref="B18:AG18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="65.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="65.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:33">
@@ -28406,13 +28407,13 @@
       <selection activeCell="AI10" sqref="AI10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="15.85546875" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" customWidth="1"/>
-    <col min="3" max="3" width="9.5703125" customWidth="1"/>
-    <col min="6" max="6" width="11.85546875" customWidth="1"/>
-    <col min="8" max="8" width="9.85546875" customWidth="1"/>
+    <col min="1" max="1" width="15.81640625" customWidth="1"/>
+    <col min="2" max="2" width="14.81640625" customWidth="1"/>
+    <col min="3" max="3" width="9.54296875" customWidth="1"/>
+    <col min="6" max="6" width="11.81640625" customWidth="1"/>
+    <col min="8" max="8" width="9.81640625" customWidth="1"/>
     <col min="13" max="13" width="12" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="12" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="12" bestFit="1" customWidth="1"/>
@@ -29159,16 +29160,16 @@
   <dimension ref="A1:AI15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G3" sqref="G3:M3"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="17.7109375" customWidth="1"/>
-    <col min="2" max="2" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.140625" customWidth="1"/>
-    <col min="4" max="4" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.7109375" customWidth="1"/>
+    <col min="1" max="1" width="17.7265625" customWidth="1"/>
+    <col min="2" max="2" width="17.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.1796875" customWidth="1"/>
+    <col min="4" max="4" width="8.54296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.7265625" customWidth="1"/>
     <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="11" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="11" bestFit="1" customWidth="1"/>
@@ -29266,12 +29267,12 @@
         <v>279</v>
       </c>
       <c r="B4">
-        <f>B3/10^6</f>
-        <v>3.2648000000000003E-2</v>
+        <f>B3*10^6</f>
+        <v>32648000000</v>
       </c>
       <c r="C4">
-        <f>C3/10^6</f>
-        <v>2.6238000000000001E-2</v>
+        <f>C3*10^6</f>
+        <v>26238000000</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -29309,12 +29310,12 @@
         <v>280</v>
       </c>
       <c r="B5">
-        <f>B4*1000</f>
-        <v>32.648000000000003</v>
+        <f>B4/1000</f>
+        <v>32648000</v>
       </c>
       <c r="C5">
-        <f>C4*1000</f>
-        <v>26.238</v>
+        <f>C4/1000</f>
+        <v>26238000</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -29353,11 +29354,11 @@
       </c>
       <c r="B6">
         <f>B5*'Conversion Factors'!$B$59</f>
-        <v>1175328000</v>
+        <v>1175328000000000</v>
       </c>
       <c r="C6">
         <f>C5*'Conversion Factors'!$B$59</f>
-        <v>944568000</v>
+        <v>944568000000000</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -29612,139 +29613,139 @@
       </c>
       <c r="B14">
         <f>B6</f>
-        <v>1175328000</v>
+        <v>1175328000000000</v>
       </c>
       <c r="C14">
         <f>B14*(1+$H$5)</f>
-        <v>1214506491.7213566</v>
+        <v>1214506491721356.5</v>
       </c>
       <c r="D14">
         <f t="shared" ref="D14:G14" si="5">C14*(1+$H$5)</f>
-        <v>1254990962.8914802</v>
+        <v>1254990962891480</v>
       </c>
       <c r="E14">
         <f t="shared" si="5"/>
-        <v>1296824947.1495094</v>
+        <v>1296824947149509.3</v>
       </c>
       <c r="F14">
         <f t="shared" si="5"/>
-        <v>1340053429.2889171</v>
+        <v>1340053429288916.8</v>
       </c>
       <c r="G14">
         <f t="shared" si="5"/>
-        <v>1384722893.6304212</v>
+        <v>1384722893630420.8</v>
       </c>
       <c r="H14">
         <f>G14*(1+$I$5)</f>
-        <v>1449342887.8482506</v>
+        <v>1449342887848250.3</v>
       </c>
       <c r="I14">
         <f t="shared" ref="I14:L14" si="6">H14*(1+$I$5)</f>
-        <v>1516978462.7804024</v>
+        <v>1516978462780402</v>
       </c>
       <c r="J14">
         <f t="shared" si="6"/>
-        <v>1587770344.6394777</v>
+        <v>1587770344639477.3</v>
       </c>
       <c r="K14">
         <f t="shared" si="6"/>
-        <v>1661865826.8199208</v>
+        <v>1661865826819920.3</v>
       </c>
       <c r="L14">
         <f t="shared" si="6"/>
-        <v>1739419076.3645723</v>
+        <v>1739419076364571.8</v>
       </c>
       <c r="M14">
         <f>L14*(1+$J$5)</f>
-        <v>1816809204.9845138</v>
+        <v>1816809204984513.3</v>
       </c>
       <c r="N14">
         <f t="shared" ref="N14:Q14" si="7">M14*(1+$J$5)</f>
-        <v>1897642570.5386672</v>
+        <v>1897642570538666.5</v>
       </c>
       <c r="O14">
         <f t="shared" si="7"/>
-        <v>1982072369.3170054</v>
+        <v>1982072369317004.8</v>
       </c>
       <c r="P14">
         <f t="shared" si="7"/>
-        <v>2070258613.6095941</v>
+        <v>2070258613609593.5</v>
       </c>
       <c r="Q14">
         <f t="shared" si="7"/>
-        <v>2162368434.9636559</v>
+        <v>2162368434963655.5</v>
       </c>
       <c r="R14">
         <f>Q14*(1+$K$5)</f>
-        <v>2254335327.7793608</v>
+        <v>2254335327779360.5</v>
       </c>
       <c r="S14">
         <f t="shared" ref="S14:V14" si="8">R14*(1+$K$5)</f>
-        <v>2350213630.5275354</v>
+        <v>2350213630527535</v>
       </c>
       <c r="T14">
         <f t="shared" si="8"/>
-        <v>2450169697.9385767</v>
+        <v>2450169697938576</v>
       </c>
       <c r="U14">
         <f t="shared" si="8"/>
-        <v>2554376959.9144449</v>
+        <v>2554376959914444</v>
       </c>
       <c r="V14">
         <f t="shared" si="8"/>
-        <v>2663016222.4401703</v>
+        <v>2663016222440169</v>
       </c>
       <c r="W14">
         <f>V14*(1+$L$5)</f>
-        <v>2782500363.6382184</v>
+        <v>2782500363638217</v>
       </c>
       <c r="X14">
         <f t="shared" ref="X14:AA14" si="9">W14*(1+$L$5)</f>
-        <v>2907345516.1127028</v>
+        <v>2907345516112701.5</v>
       </c>
       <c r="Y14">
         <f t="shared" si="9"/>
-        <v>3037792217.5753059</v>
+        <v>3037792217575304.5</v>
       </c>
       <c r="Z14">
         <f t="shared" si="9"/>
-        <v>3174091798.1773744</v>
+        <v>3174091798177372.5</v>
       </c>
       <c r="AA14">
         <f t="shared" si="9"/>
-        <v>3316506864.7448153</v>
+        <v>3316506864744813</v>
       </c>
       <c r="AB14">
         <f>AA14*(1+$M$5)</f>
-        <v>3474467101.4868736</v>
+        <v>3474467101486871.5</v>
       </c>
       <c r="AC14">
         <f t="shared" ref="AC14:AF14" si="10">AB14*(1+$M$5)</f>
-        <v>3639950746.866148</v>
+        <v>3639950746866146</v>
       </c>
       <c r="AD14">
         <f t="shared" si="10"/>
-        <v>3813316129.5271754</v>
+        <v>3813316129527173.5</v>
       </c>
       <c r="AE14">
         <f t="shared" si="10"/>
-        <v>3994938644.7692084</v>
+        <v>3994938644769206.5</v>
       </c>
       <c r="AF14">
         <f t="shared" si="10"/>
-        <v>4185211567.4053259</v>
+        <v>4185211567405324</v>
       </c>
       <c r="AG14">
         <f>AF14</f>
-        <v>4185211567.4053259</v>
+        <v>4185211567405324</v>
       </c>
       <c r="AH14">
         <f t="shared" ref="AH14:AI14" si="11">AG14</f>
-        <v>4185211567.4053259</v>
+        <v>4185211567405324</v>
       </c>
       <c r="AI14">
         <f t="shared" si="11"/>
-        <v>4185211567.4053259</v>
+        <v>4185211567405324</v>
       </c>
     </row>
     <row r="15" spans="1:35">
@@ -29753,139 +29754,139 @@
       </c>
       <c r="B15">
         <f>C6</f>
-        <v>944568000</v>
+        <v>944568000000000</v>
       </c>
       <c r="C15">
         <f>B15*(1+$H$9)</f>
-        <v>978485825.88333893</v>
+        <v>978485825883339</v>
       </c>
       <c r="D15">
         <f t="shared" ref="D15:G15" si="12">C15*(1+$H$9)</f>
-        <v>1013621583.0460061</v>
+        <v>1013621583046006.1</v>
       </c>
       <c r="E15">
         <f t="shared" si="12"/>
-        <v>1050019005.323014</v>
+        <v>1050019005323014</v>
       </c>
       <c r="F15">
         <f t="shared" si="12"/>
-        <v>1087723396.9568009</v>
+        <v>1087723396956800.9</v>
       </c>
       <c r="G15">
         <f t="shared" si="12"/>
-        <v>1126781688.9878826</v>
+        <v>1126781688987882.5</v>
       </c>
       <c r="H15">
         <f>G15*(1+$I$9)</f>
-        <v>1138906138.2336495</v>
+        <v>1138906138233649.5</v>
       </c>
       <c r="I15">
         <f t="shared" ref="I15:L15" si="13">H15*(1+$I$9)</f>
-        <v>1151161049.5475791</v>
+        <v>1151161049547579</v>
       </c>
       <c r="J15">
         <f t="shared" si="13"/>
-        <v>1163547826.7337439</v>
+        <v>1163547826733743.8</v>
       </c>
       <c r="K15">
         <f t="shared" si="13"/>
-        <v>1176067888.7014952</v>
+        <v>1176067888701495</v>
       </c>
       <c r="L15">
         <f t="shared" si="13"/>
-        <v>1188722669.6279988</v>
+        <v>1188722669627998.8</v>
       </c>
       <c r="M15">
         <f>L15*(1+$J$9)</f>
-        <v>1205496447.1504569</v>
+        <v>1205496447150456.8</v>
       </c>
       <c r="N15">
         <f t="shared" ref="N15:Q15" si="14">M15*(1+$J$9)</f>
-        <v>1222506915.3826673</v>
+        <v>1222506915382667</v>
       </c>
       <c r="O15">
         <f t="shared" si="14"/>
-        <v>1239757414.2098768</v>
+        <v>1239757414209876.5</v>
       </c>
       <c r="P15">
         <f t="shared" si="14"/>
-        <v>1257251330.6456439</v>
+        <v>1257251330645643.8</v>
       </c>
       <c r="Q15">
         <f t="shared" si="14"/>
-        <v>1274992099.4968545</v>
+        <v>1274992099496854.3</v>
       </c>
       <c r="R15">
         <f>Q15*(1+$K$9)</f>
-        <v>1274379003.3355594</v>
+        <v>1274379003335559</v>
       </c>
       <c r="S15">
         <f t="shared" ref="S15:V15" si="15">R15*(1+$K$9)</f>
-        <v>1273766201.9893482</v>
+        <v>1273766201989347.8</v>
       </c>
       <c r="T15">
         <f t="shared" si="15"/>
-        <v>1273153695.3164556</v>
+        <v>1273153695316455</v>
       </c>
       <c r="U15">
         <f t="shared" si="15"/>
-        <v>1272541483.175184</v>
+        <v>1272541483175183.5</v>
       </c>
       <c r="V15">
         <f t="shared" si="15"/>
-        <v>1271929565.4239042</v>
+        <v>1271929565423903.8</v>
       </c>
       <c r="W15">
         <f>V15*(1+$L$9)</f>
-        <v>1260606340.2859473</v>
+        <v>1260606340285946.8</v>
       </c>
       <c r="X15">
         <f t="shared" ref="X15:AA15" si="16">W15*(1+$L$9)</f>
-        <v>1249383919.0218921</v>
+        <v>1249383919021891.5</v>
       </c>
       <c r="Y15">
         <f t="shared" si="16"/>
-        <v>1238261404.2353811</v>
+        <v>1238261404235380.5</v>
       </c>
       <c r="Z15">
         <f t="shared" si="16"/>
-        <v>1227237906.5190377</v>
+        <v>1227237906519037.3</v>
       </c>
       <c r="AA15">
         <f t="shared" si="16"/>
-        <v>1216312544.3833454</v>
+        <v>1216312544383344.8</v>
       </c>
       <c r="AB15">
         <f>AA15*(1+$M$9)</f>
-        <v>1167620883.0635505</v>
+        <v>1167620883063550</v>
       </c>
       <c r="AC15">
         <f t="shared" ref="AC15:AF15" si="17">AB15*(1+$M$9)</f>
-        <v>1120878455.8390791</v>
+        <v>1120878455839078.6</v>
       </c>
       <c r="AD15">
         <f t="shared" si="17"/>
-        <v>1076007230.5899463</v>
+        <v>1076007230589945.8</v>
       </c>
       <c r="AE15">
         <f t="shared" si="17"/>
-        <v>1032932298.9932337</v>
+        <v>1032932298993233.3</v>
       </c>
       <c r="AF15">
         <f t="shared" si="17"/>
-        <v>991581751.47063565</v>
+        <v>991581751470635.25</v>
       </c>
       <c r="AG15">
         <f>AF15</f>
-        <v>991581751.47063565</v>
+        <v>991581751470635.25</v>
       </c>
       <c r="AH15">
         <f t="shared" ref="AH15:AI15" si="18">AG15</f>
-        <v>991581751.47063565</v>
+        <v>991581751470635.25</v>
       </c>
       <c r="AI15">
         <f t="shared" si="18"/>
-        <v>991581751.47063565</v>
+        <v>991581751470635.25</v>
       </c>
     </row>
   </sheetData>
@@ -29901,14 +29902,14 @@
       <selection activeCell="B31" sqref="B31:AG31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" customWidth="1"/>
-    <col min="2" max="2" width="16.85546875" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" customWidth="1"/>
-    <col min="4" max="4" width="22.7109375" customWidth="1"/>
-    <col min="6" max="6" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.140625" customWidth="1"/>
+    <col min="1" max="1" width="10.54296875" customWidth="1"/>
+    <col min="2" max="2" width="16.81640625" customWidth="1"/>
+    <col min="3" max="3" width="15.54296875" customWidth="1"/>
+    <col min="4" max="4" width="22.7265625" customWidth="1"/>
+    <col min="6" max="6" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.1796875" customWidth="1"/>
     <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="12" bestFit="1" customWidth="1"/>
@@ -31038,18 +31039,18 @@
       <selection activeCell="J34" sqref="J34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
-    <col min="2" max="2" width="11.140625" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" customWidth="1"/>
+    <col min="2" max="2" width="11.1796875" customWidth="1"/>
+    <col min="3" max="3" width="11.54296875" customWidth="1"/>
     <col min="4" max="4" width="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="4.140625" customWidth="1"/>
-    <col min="6" max="6" width="21.5703125" customWidth="1"/>
+    <col min="5" max="5" width="4.1796875" customWidth="1"/>
+    <col min="6" max="6" width="21.54296875" customWidth="1"/>
     <col min="7" max="7" width="11" customWidth="1"/>
     <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.85546875" customWidth="1"/>
-    <col min="18" max="18" width="9.42578125" customWidth="1"/>
+    <col min="13" max="13" width="9.81640625" customWidth="1"/>
+    <col min="18" max="18" width="9.453125" customWidth="1"/>
     <col min="23" max="23" width="12" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="12" bestFit="1" customWidth="1"/>
     <col min="33" max="33" width="12" bestFit="1" customWidth="1"/>
@@ -31119,25 +31120,25 @@
       <c r="D3">
         <v>1.05</v>
       </c>
-      <c r="H3" s="97">
+      <c r="H3" s="95">
         <v>3408.4500000000003</v>
       </c>
-      <c r="I3" s="97">
+      <c r="I3" s="95">
         <v>4203.6000000000004</v>
       </c>
-      <c r="J3" s="97">
+      <c r="J3" s="95">
         <v>4887.1500000000005</v>
       </c>
-      <c r="K3" s="97">
+      <c r="K3" s="95">
         <v>5356.8</v>
       </c>
-      <c r="L3" s="97">
+      <c r="L3" s="95">
         <v>5538.1500000000005</v>
       </c>
-      <c r="M3" s="97">
+      <c r="M3" s="95">
         <v>5528.85</v>
       </c>
-      <c r="N3" s="97">
+      <c r="N3" s="95">
         <v>5380.05</v>
       </c>
     </row>
@@ -31241,25 +31242,25 @@
       <c r="K6" s="56"/>
     </row>
     <row r="7" spans="1:40" ht="15" customHeight="1">
-      <c r="H7" s="98">
+      <c r="H7" s="96">
         <v>-876.28625387650709</v>
       </c>
-      <c r="I7" s="98">
+      <c r="I7" s="96">
         <v>-1132.7566268697301</v>
       </c>
-      <c r="J7" s="98">
+      <c r="J7" s="96">
         <v>-1348.9801264516409</v>
       </c>
-      <c r="K7" s="98">
+      <c r="K7" s="96">
         <v>-1632.1478019750093</v>
       </c>
-      <c r="L7" s="98">
+      <c r="L7" s="96">
         <v>-2122.672138171396</v>
       </c>
-      <c r="M7" s="98">
+      <c r="M7" s="96">
         <v>-2755.5542138460569</v>
       </c>
-      <c r="N7" s="98">
+      <c r="N7" s="96">
         <v>-3300.298451450094</v>
       </c>
     </row>
@@ -32141,14 +32142,14 @@
       <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="43.7109375" customWidth="1"/>
+    <col min="1" max="1" width="43.7265625" customWidth="1"/>
     <col min="2" max="3" width="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.85546875" customWidth="1"/>
+    <col min="4" max="4" width="10.81640625" customWidth="1"/>
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="59.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="59.54296875" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="12" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="12" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="12" bestFit="1" customWidth="1"/>

</xml_diff>